<commit_message>
bugfix excel template WM 2022
</commit_message>
<xml_diff>
--- a/extra/excel_templates/WM_2022.xlsx
+++ b/extra/excel_templates/WM_2022.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jörn\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sync\dev\1_Github\fredbet\extra\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{327F6959-1505-BC48-8033-252AD2C70DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BB5A41E-4915-41F5-96C6-1F06B737AFE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matches" sheetId="1" r:id="rId1"/>
@@ -1211,20 +1211,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E452"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.1953125" customWidth="1"/>
-    <col min="2" max="2" width="25.2890625" customWidth="1"/>
-    <col min="3" max="3" width="24.078125" customWidth="1"/>
-    <col min="4" max="4" width="21.65625" customWidth="1"/>
-    <col min="5" max="5" width="28.515625" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>116</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>72</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>194</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>206</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>136</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>182</v>
       </c>
@@ -1360,7 +1360,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>214</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>208</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>116</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>154</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>82</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1632,7 +1632,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>206</v>
       </c>
@@ -1649,12 +1649,12 @@
         <v>244</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>98</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>170</v>
       </c>
       <c r="C26" t="s">
         <v>219</v>
@@ -1666,7 +1666,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>5</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>14</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>48</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>101</v>
       </c>
@@ -1751,7 +1751,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>208</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>18</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>154</v>
       </c>
@@ -1802,7 +1802,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>211</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>96</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>82</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>30</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>117</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>17</v>
       </c>
@@ -1921,7 +1921,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>168</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>170</v>
       </c>
@@ -1972,7 +1972,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>98</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>101</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>158</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>231</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>234</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>230</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>228</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>235</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>248</v>
       </c>
@@ -2159,7 +2159,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>237</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>250</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>260</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>262</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>264</v>
       </c>
@@ -2244,7 +2244,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>266</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>253</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>254</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>256</v>
       </c>
@@ -2312,7 +2312,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>258</v>
       </c>
@@ -2329,1165 +2329,1165 @@
         <v>244</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D75" s="2"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D86" s="2"/>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D87" s="2"/>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D93" s="2"/>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D94" s="2"/>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D95" s="2"/>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D96" s="2"/>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D97" s="2"/>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D98" s="2"/>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D99" s="2"/>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D100" s="2"/>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D101" s="2"/>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D102" s="2"/>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D103" s="2"/>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D104" s="2"/>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D105" s="2"/>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D106" s="2"/>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D107" s="2"/>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D109" s="2"/>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D110" s="2"/>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D111" s="2"/>
     </row>
-    <row r="112" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="112" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D112" s="2"/>
     </row>
-    <row r="113" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="113" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D113" s="2"/>
     </row>
-    <row r="114" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="114" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D114" s="2"/>
     </row>
-    <row r="115" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="115" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D115" s="2"/>
     </row>
-    <row r="116" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D116" s="2"/>
     </row>
-    <row r="117" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D117" s="2"/>
     </row>
-    <row r="118" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="118" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D118" s="2"/>
     </row>
-    <row r="119" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="119" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D119" s="2"/>
     </row>
-    <row r="120" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="120" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D120" s="2"/>
     </row>
-    <row r="121" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="121" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D121" s="2"/>
     </row>
-    <row r="122" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="122" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D122" s="2"/>
     </row>
-    <row r="123" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="123" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D123" s="2"/>
     </row>
-    <row r="124" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="124" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D124" s="2"/>
     </row>
-    <row r="125" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="125" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D125" s="2"/>
     </row>
-    <row r="126" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="126" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D126" s="2"/>
     </row>
-    <row r="127" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="127" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D127" s="2"/>
     </row>
-    <row r="128" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="128" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D128" s="2"/>
     </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D129" s="2"/>
     </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D130" s="2"/>
     </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D131" s="2"/>
     </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D132" s="2"/>
     </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D133" s="2"/>
     </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D134" s="2"/>
     </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D135" s="2"/>
     </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D136" s="2"/>
     </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D137" s="2"/>
     </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D138" s="2"/>
     </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D139" s="2"/>
     </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D140" s="2"/>
     </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D141" s="2"/>
     </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D142" s="2"/>
     </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D143" s="2"/>
     </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D144" s="2"/>
     </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D145" s="2"/>
     </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D146" s="2"/>
     </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D147" s="2"/>
     </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D148" s="2"/>
     </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D149" s="2"/>
     </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D150" s="2"/>
     </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D151" s="2"/>
     </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D152" s="2"/>
     </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D153" s="2"/>
     </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D154" s="2"/>
     </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D155" s="2"/>
     </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D156" s="2"/>
     </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D157" s="2"/>
     </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="158" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D158" s="2"/>
     </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D159" s="2"/>
     </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D160" s="2"/>
     </row>
-    <row r="161" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="161" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D161" s="2"/>
     </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="162" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D162" s="2"/>
     </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="163" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D163" s="2"/>
     </row>
-    <row r="164" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="164" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D164" s="2"/>
     </row>
-    <row r="165" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="165" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D165" s="2"/>
     </row>
-    <row r="166" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="166" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D166" s="2"/>
     </row>
-    <row r="167" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="167" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D167" s="2"/>
     </row>
-    <row r="168" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="168" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D168" s="2"/>
     </row>
-    <row r="169" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="169" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D169" s="2"/>
     </row>
-    <row r="170" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="170" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D170" s="2"/>
     </row>
-    <row r="171" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="171" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D171" s="2"/>
     </row>
-    <row r="172" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="172" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D172" s="2"/>
     </row>
-    <row r="173" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="173" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D173" s="2"/>
     </row>
-    <row r="174" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="174" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D174" s="2"/>
     </row>
-    <row r="175" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="175" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D175" s="2"/>
     </row>
-    <row r="176" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="176" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D176" s="2"/>
     </row>
-    <row r="177" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="177" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D177" s="2"/>
     </row>
-    <row r="178" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="178" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D178" s="2"/>
     </row>
-    <row r="179" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="179" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D179" s="2"/>
     </row>
-    <row r="180" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="180" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D180" s="2"/>
     </row>
-    <row r="181" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="181" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D181" s="2"/>
     </row>
-    <row r="182" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="182" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D182" s="2"/>
     </row>
-    <row r="183" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="183" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D183" s="2"/>
     </row>
-    <row r="184" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="184" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D184" s="2"/>
     </row>
-    <row r="185" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="185" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D185" s="2"/>
     </row>
-    <row r="186" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="186" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D186" s="2"/>
     </row>
-    <row r="187" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="187" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D187" s="2"/>
     </row>
-    <row r="188" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="188" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D188" s="2"/>
     </row>
-    <row r="189" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="189" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D189" s="2"/>
     </row>
-    <row r="190" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="190" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D190" s="2"/>
     </row>
-    <row r="191" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="191" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D191" s="2"/>
     </row>
-    <row r="192" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="192" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D192" s="2"/>
     </row>
-    <row r="193" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D193" s="2"/>
     </row>
-    <row r="194" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="194" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D194" s="2"/>
     </row>
-    <row r="195" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="195" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D195" s="2"/>
     </row>
-    <row r="196" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="196" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D196" s="2"/>
     </row>
-    <row r="197" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="197" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D197" s="2"/>
     </row>
-    <row r="198" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="198" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D198" s="2"/>
     </row>
-    <row r="199" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="199" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D199" s="2"/>
     </row>
-    <row r="200" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="200" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D200" s="2"/>
     </row>
-    <row r="201" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="201" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D201" s="2"/>
     </row>
-    <row r="202" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="202" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D202" s="2"/>
     </row>
-    <row r="203" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="203" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D203" s="2"/>
     </row>
-    <row r="204" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="204" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D204" s="2"/>
     </row>
-    <row r="205" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="205" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D205" s="2"/>
     </row>
-    <row r="206" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="206" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D206" s="2"/>
     </row>
-    <row r="207" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="207" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D207" s="2"/>
     </row>
-    <row r="208" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="208" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D208" s="2"/>
     </row>
-    <row r="209" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="209" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D209" s="2"/>
     </row>
-    <row r="210" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="210" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D210" s="2"/>
     </row>
-    <row r="211" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="211" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D211" s="2"/>
     </row>
-    <row r="212" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="212" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D212" s="2"/>
     </row>
-    <row r="213" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="213" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D213" s="2"/>
     </row>
-    <row r="214" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="214" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D214" s="2"/>
     </row>
-    <row r="215" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="215" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D215" s="2"/>
     </row>
-    <row r="216" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="216" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D216" s="2"/>
     </row>
-    <row r="217" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="217" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D217" s="2"/>
     </row>
-    <row r="218" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="218" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D218" s="2"/>
     </row>
-    <row r="219" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="219" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D219" s="2"/>
     </row>
-    <row r="220" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="220" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D220" s="2"/>
     </row>
-    <row r="221" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="221" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D221" s="2"/>
     </row>
-    <row r="222" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="222" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D222" s="2"/>
     </row>
-    <row r="223" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="223" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D223" s="2"/>
     </row>
-    <row r="224" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="224" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D224" s="2"/>
     </row>
-    <row r="225" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="225" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D225" s="2"/>
     </row>
-    <row r="226" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="226" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D226" s="2"/>
     </row>
-    <row r="227" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="227" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D227" s="2"/>
     </row>
-    <row r="228" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="228" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D228" s="2"/>
     </row>
-    <row r="229" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="229" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D229" s="2"/>
     </row>
-    <row r="230" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="230" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D230" s="2"/>
     </row>
-    <row r="231" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="231" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D231" s="2"/>
     </row>
-    <row r="232" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="232" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D232" s="2"/>
     </row>
-    <row r="233" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="233" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D233" s="2"/>
     </row>
-    <row r="234" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="234" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D234" s="2"/>
     </row>
-    <row r="235" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="235" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D235" s="2"/>
     </row>
-    <row r="236" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="236" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D236" s="2"/>
     </row>
-    <row r="237" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="237" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D237" s="2"/>
     </row>
-    <row r="238" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="238" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D238" s="2"/>
     </row>
-    <row r="239" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="239" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D239" s="2"/>
     </row>
-    <row r="240" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="240" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D240" s="2"/>
     </row>
-    <row r="241" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="241" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D241" s="2"/>
     </row>
-    <row r="242" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="242" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D242" s="2"/>
     </row>
-    <row r="243" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="243" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D243" s="2"/>
     </row>
-    <row r="244" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="244" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D244" s="2"/>
     </row>
-    <row r="245" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="245" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D245" s="2"/>
     </row>
-    <row r="246" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="246" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D246" s="2"/>
     </row>
-    <row r="247" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="247" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D247" s="2"/>
     </row>
-    <row r="248" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="248" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D248" s="2"/>
     </row>
-    <row r="249" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="249" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D249" s="2"/>
     </row>
-    <row r="250" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="250" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D250" s="2"/>
     </row>
-    <row r="251" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="251" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D251" s="2"/>
     </row>
-    <row r="252" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="252" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D252" s="2"/>
     </row>
-    <row r="253" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="253" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D253" s="2"/>
     </row>
-    <row r="254" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="254" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D254" s="2"/>
     </row>
-    <row r="255" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="255" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D255" s="2"/>
     </row>
-    <row r="256" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="256" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D256" s="2"/>
     </row>
-    <row r="257" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="257" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D257" s="2"/>
     </row>
-    <row r="258" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="258" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D258" s="2"/>
     </row>
-    <row r="259" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="259" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D259" s="2"/>
     </row>
-    <row r="260" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="260" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D260" s="2"/>
     </row>
-    <row r="261" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="261" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D261" s="2"/>
     </row>
-    <row r="262" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="262" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D262" s="2"/>
     </row>
-    <row r="263" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="263" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D263" s="2"/>
     </row>
-    <row r="264" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="264" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D264" s="2"/>
     </row>
-    <row r="265" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="265" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D265" s="2"/>
     </row>
-    <row r="266" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="266" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D266" s="2"/>
     </row>
-    <row r="267" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="267" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D267" s="2"/>
     </row>
-    <row r="268" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="268" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D268" s="2"/>
     </row>
-    <row r="269" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="269" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D269" s="2"/>
     </row>
-    <row r="270" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="270" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D270" s="2"/>
     </row>
-    <row r="271" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="271" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D271" s="2"/>
     </row>
-    <row r="272" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="272" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D272" s="2"/>
     </row>
-    <row r="273" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="273" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D273" s="2"/>
     </row>
-    <row r="274" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="274" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D274" s="2"/>
     </row>
-    <row r="275" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="275" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D275" s="2"/>
     </row>
-    <row r="276" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="276" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D276" s="2"/>
     </row>
-    <row r="277" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="277" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D277" s="2"/>
     </row>
-    <row r="278" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="278" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D278" s="2"/>
     </row>
-    <row r="279" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="279" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D279" s="2"/>
     </row>
-    <row r="280" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="280" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D280" s="2"/>
     </row>
-    <row r="281" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="281" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D281" s="2"/>
     </row>
-    <row r="282" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="282" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D282" s="2"/>
     </row>
-    <row r="283" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="283" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D283" s="2"/>
     </row>
-    <row r="284" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="284" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D284" s="2"/>
     </row>
-    <row r="285" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="285" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D285" s="2"/>
     </row>
-    <row r="286" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="286" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D286" s="2"/>
     </row>
-    <row r="287" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="287" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D287" s="2"/>
     </row>
-    <row r="288" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="288" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D288" s="2"/>
     </row>
-    <row r="289" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="289" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D289" s="2"/>
     </row>
-    <row r="290" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="290" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D290" s="2"/>
     </row>
-    <row r="291" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="291" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D291" s="2"/>
     </row>
-    <row r="292" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="292" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D292" s="2"/>
     </row>
-    <row r="293" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="293" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D293" s="2"/>
     </row>
-    <row r="294" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="294" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D294" s="2"/>
     </row>
-    <row r="295" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="295" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D295" s="2"/>
     </row>
-    <row r="296" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="296" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D296" s="2"/>
     </row>
-    <row r="297" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="297" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D297" s="2"/>
     </row>
-    <row r="298" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="298" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D298" s="2"/>
     </row>
-    <row r="299" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="299" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D299" s="2"/>
     </row>
-    <row r="300" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="300" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D300" s="2"/>
     </row>
-    <row r="301" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="301" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D301" s="2"/>
     </row>
-    <row r="302" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="302" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D302" s="2"/>
     </row>
-    <row r="303" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="303" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D303" s="2"/>
     </row>
-    <row r="304" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="304" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D304" s="2"/>
     </row>
-    <row r="305" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="305" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D305" s="2"/>
     </row>
-    <row r="306" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="306" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D306" s="2"/>
     </row>
-    <row r="307" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="307" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D307" s="2"/>
     </row>
-    <row r="308" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="308" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D308" s="2"/>
     </row>
-    <row r="309" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="309" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D309" s="2"/>
     </row>
-    <row r="310" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="310" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D310" s="2"/>
     </row>
-    <row r="311" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="311" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D311" s="2"/>
     </row>
-    <row r="312" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="312" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D312" s="2"/>
     </row>
-    <row r="313" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="313" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D313" s="2"/>
     </row>
-    <row r="314" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="314" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D314" s="2"/>
     </row>
-    <row r="315" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="315" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D315" s="2"/>
     </row>
-    <row r="316" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="316" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D316" s="2"/>
     </row>
-    <row r="317" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="317" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D317" s="2"/>
     </row>
-    <row r="318" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="318" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D318" s="2"/>
     </row>
-    <row r="319" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="319" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D319" s="2"/>
     </row>
-    <row r="320" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="320" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D320" s="2"/>
     </row>
-    <row r="321" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="321" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D321" s="2"/>
     </row>
-    <row r="322" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="322" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D322" s="2"/>
     </row>
-    <row r="323" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="323" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D323" s="2"/>
     </row>
-    <row r="324" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="324" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D324" s="2"/>
     </row>
-    <row r="325" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="325" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D325" s="2"/>
     </row>
-    <row r="326" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="326" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D326" s="2"/>
     </row>
-    <row r="327" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="327" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D327" s="2"/>
     </row>
-    <row r="328" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="328" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D328" s="2"/>
     </row>
-    <row r="329" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="329" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D329" s="2"/>
     </row>
-    <row r="330" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="330" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D330" s="2"/>
     </row>
-    <row r="331" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="331" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D331" s="2"/>
     </row>
-    <row r="332" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="332" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D332" s="2"/>
     </row>
-    <row r="333" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="333" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D333" s="2"/>
     </row>
-    <row r="334" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="334" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D334" s="2"/>
     </row>
-    <row r="335" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="335" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D335" s="2"/>
     </row>
-    <row r="336" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="336" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D336" s="2"/>
     </row>
-    <row r="337" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="337" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D337" s="2"/>
     </row>
-    <row r="338" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="338" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D338" s="2"/>
     </row>
-    <row r="339" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="339" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D339" s="2"/>
     </row>
-    <row r="340" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="340" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D340" s="2"/>
     </row>
-    <row r="341" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="341" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D341" s="2"/>
     </row>
-    <row r="342" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="342" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D342" s="2"/>
     </row>
-    <row r="343" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="343" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D343" s="2"/>
     </row>
-    <row r="344" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="344" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D344" s="2"/>
     </row>
-    <row r="345" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="345" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D345" s="2"/>
     </row>
-    <row r="346" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="346" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D346" s="2"/>
     </row>
-    <row r="347" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="347" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D347" s="2"/>
     </row>
-    <row r="348" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="348" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D348" s="2"/>
     </row>
-    <row r="349" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="349" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D349" s="2"/>
     </row>
-    <row r="350" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="350" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D350" s="2"/>
     </row>
-    <row r="351" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="351" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D351" s="2"/>
     </row>
-    <row r="352" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="352" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D352" s="2"/>
     </row>
-    <row r="353" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="353" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D353" s="2"/>
     </row>
-    <row r="354" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="354" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D354" s="2"/>
     </row>
-    <row r="355" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="355" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D355" s="2"/>
     </row>
-    <row r="356" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="356" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D356" s="2"/>
     </row>
-    <row r="357" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="357" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D357" s="2"/>
     </row>
-    <row r="358" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="358" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D358" s="2"/>
     </row>
-    <row r="359" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="359" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D359" s="2"/>
     </row>
-    <row r="360" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="360" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D360" s="2"/>
     </row>
-    <row r="361" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="361" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D361" s="2"/>
     </row>
-    <row r="362" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="362" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D362" s="2"/>
     </row>
-    <row r="363" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="363" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D363" s="2"/>
     </row>
-    <row r="364" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="364" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D364" s="2"/>
     </row>
-    <row r="365" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="365" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D365" s="2"/>
     </row>
-    <row r="366" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="366" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D366" s="2"/>
     </row>
-    <row r="367" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="367" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D367" s="2"/>
     </row>
-    <row r="368" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="368" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D368" s="2"/>
     </row>
-    <row r="369" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="369" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D369" s="2"/>
     </row>
-    <row r="370" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="370" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D370" s="2"/>
     </row>
-    <row r="371" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="371" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D371" s="2"/>
     </row>
-    <row r="372" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="372" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D372" s="2"/>
     </row>
-    <row r="373" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="373" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D373" s="2"/>
     </row>
-    <row r="374" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="374" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D374" s="2"/>
     </row>
-    <row r="375" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="375" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D375" s="2"/>
     </row>
-    <row r="376" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="376" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D376" s="2"/>
     </row>
-    <row r="377" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="377" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D377" s="2"/>
     </row>
-    <row r="378" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="378" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D378" s="2"/>
     </row>
-    <row r="379" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="379" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D379" s="2"/>
     </row>
-    <row r="380" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="380" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D380" s="2"/>
     </row>
-    <row r="381" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="381" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D381" s="2"/>
     </row>
-    <row r="382" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="382" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D382" s="2"/>
     </row>
-    <row r="383" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="383" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D383" s="2"/>
     </row>
-    <row r="384" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="384" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D384" s="2"/>
     </row>
-    <row r="385" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="385" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D385" s="2"/>
     </row>
-    <row r="386" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="386" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D386" s="2"/>
     </row>
-    <row r="387" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="387" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D387" s="2"/>
     </row>
-    <row r="388" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="388" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D388" s="2"/>
     </row>
-    <row r="389" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="389" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D389" s="2"/>
     </row>
-    <row r="390" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="390" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D390" s="2"/>
     </row>
-    <row r="391" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="391" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D391" s="2"/>
     </row>
-    <row r="392" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="392" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D392" s="2"/>
     </row>
-    <row r="393" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="393" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D393" s="2"/>
     </row>
-    <row r="394" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="394" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D394" s="2"/>
     </row>
-    <row r="395" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="395" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D395" s="2"/>
     </row>
-    <row r="396" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="396" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D396" s="2"/>
     </row>
-    <row r="397" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="397" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D397" s="2"/>
     </row>
-    <row r="398" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="398" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D398" s="2"/>
     </row>
-    <row r="399" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="399" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D399" s="2"/>
     </row>
-    <row r="400" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="400" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D400" s="2"/>
     </row>
-    <row r="401" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="401" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D401" s="2"/>
     </row>
-    <row r="402" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="402" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D402" s="2"/>
     </row>
-    <row r="403" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="403" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D403" s="2"/>
     </row>
-    <row r="404" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="404" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D404" s="2"/>
     </row>
-    <row r="405" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="405" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D405" s="2"/>
     </row>
-    <row r="406" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="406" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D406" s="2"/>
     </row>
-    <row r="407" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="407" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D407" s="2"/>
     </row>
-    <row r="408" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="408" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D408" s="2"/>
     </row>
-    <row r="409" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="409" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D409" s="2"/>
     </row>
-    <row r="410" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="410" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D410" s="2"/>
     </row>
-    <row r="411" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="411" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D411" s="2"/>
     </row>
-    <row r="412" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="412" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D412" s="2"/>
     </row>
-    <row r="413" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="413" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D413" s="2"/>
     </row>
-    <row r="414" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="414" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D414" s="2"/>
     </row>
-    <row r="415" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="415" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D415" s="2"/>
     </row>
-    <row r="416" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="416" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D416" s="2"/>
     </row>
-    <row r="417" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="417" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D417" s="2"/>
     </row>
-    <row r="418" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="418" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D418" s="2"/>
     </row>
-    <row r="419" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="419" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D419" s="2"/>
     </row>
-    <row r="420" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="420" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D420" s="2"/>
     </row>
-    <row r="421" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="421" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D421" s="2"/>
     </row>
-    <row r="422" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="422" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D422" s="2"/>
     </row>
-    <row r="423" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="423" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D423" s="2"/>
     </row>
-    <row r="424" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="424" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D424" s="2"/>
     </row>
-    <row r="425" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="425" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D425" s="2"/>
     </row>
-    <row r="426" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="426" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D426" s="2"/>
     </row>
-    <row r="427" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="427" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D427" s="2"/>
     </row>
-    <row r="428" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="428" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D428" s="2"/>
     </row>
-    <row r="429" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="429" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D429" s="2"/>
     </row>
-    <row r="430" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="430" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D430" s="2"/>
     </row>
-    <row r="431" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="431" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D431" s="2"/>
     </row>
-    <row r="432" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="432" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D432" s="2"/>
     </row>
-    <row r="433" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="433" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D433" s="2"/>
     </row>
-    <row r="434" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="434" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D434" s="2"/>
     </row>
-    <row r="435" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="435" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D435" s="2"/>
     </row>
-    <row r="436" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="436" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D436" s="2"/>
     </row>
-    <row r="437" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="437" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D437" s="2"/>
     </row>
-    <row r="438" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="438" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D438" s="2"/>
     </row>
-    <row r="439" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="439" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D439" s="2"/>
     </row>
-    <row r="440" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="440" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D440" s="2"/>
     </row>
-    <row r="441" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="441" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D441" s="2"/>
     </row>
-    <row r="442" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="442" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D442" s="2"/>
     </row>
-    <row r="443" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="443" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D443" s="2"/>
     </row>
-    <row r="444" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="444" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D444" s="2"/>
     </row>
-    <row r="445" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="445" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D445" s="2"/>
     </row>
-    <row r="446" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="446" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D446" s="2"/>
     </row>
-    <row r="447" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="447" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D447" s="2"/>
     </row>
-    <row r="448" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="448" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D448" s="2"/>
     </row>
-    <row r="449" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="449" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D449" s="2"/>
     </row>
-    <row r="450" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="450" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D450" s="2"/>
     </row>
-    <row r="451" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="451" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D451" s="2"/>
     </row>
-    <row r="452" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="452" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D452" s="2"/>
     </row>
   </sheetData>
@@ -3523,1057 +3523,1057 @@
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.98046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>84</v>
       </c>
@@ -4594,72 +4594,72 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76171875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>226</v>
       </c>

</xml_diff>